<commit_message>
Updated concept normalization results based on revision
</commit_message>
<xml_diff>
--- a/Output_Folders/Concept_Norm_Files/Open_NMT_experiment_results_training.xlsx
+++ b/Output_Folders/Concept_Norm_Files/Open_NMT_experiment_results_training.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MaylaB/Dropbox/Documents/0_Thesis_stuff-Larry_Sonia/Negacy_seq_2_seq_NER_model/ConceptRecognition/Concept_Norm_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0F83C9-C150-1E4F-8B4F-9780235B61CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994589E9-7DE3-B84F-87FB-1A151CE634BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16600" activeTab="2" xr2:uid="{82E14A74-B419-6B4E-8DDF-2A3AFADE285A}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16640" firstSheet="1" activeTab="5" xr2:uid="{82E14A74-B419-6B4E-8DDF-2A3AFADE285A}"/>
   </bookViews>
   <sheets>
     <sheet name="full files" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -180,12 +180,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -196,6 +233,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1399,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB7C19D-576A-6E41-9BE9-ADE7FC475471}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,7 +2240,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:K8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2604,13 +2644,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793AE9D8-2AAC-D542-9E13-A5F268222342}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -2632,7 +2675,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -2653,34 +2696,34 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>10727</v>
+        <v>97712</v>
       </c>
       <c r="C2" s="4">
-        <v>0.92</v>
+        <v>0.51</v>
       </c>
       <c r="D2" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G2" s="6">
         <v>0.08</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.93</v>
-      </c>
-      <c r="F2" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.14000000000000001</v>
-      </c>
       <c r="H2">
-        <v>1280</v>
+        <v>87791</v>
       </c>
       <c r="I2">
-        <v>0.94</v>
+        <v>0.47</v>
       </c>
       <c r="J2">
-        <v>0.06</v>
+        <v>0.53</v>
       </c>
       <c r="K2">
-        <v>1.43</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2688,13 +2731,13 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>5505</v>
+        <v>8953</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -2702,20 +2745,20 @@
       <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
-        <v>0</v>
+      <c r="G3" s="6">
+        <v>0.01</v>
       </c>
       <c r="H3">
-        <v>685</v>
+        <v>4047</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2723,7 +2766,7 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>91058</v>
+        <v>91252</v>
       </c>
       <c r="C4" s="4">
         <v>0.73</v>
@@ -2737,11 +2780,11 @@
       <c r="F4" s="4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="6">
         <v>0.02</v>
       </c>
       <c r="H4">
-        <v>80402</v>
+        <v>80532</v>
       </c>
       <c r="I4">
         <v>0.71</v>
@@ -2758,7 +2801,7 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>13183</v>
+        <v>13270</v>
       </c>
       <c r="C5" s="4">
         <v>0.97</v>
@@ -2772,11 +2815,11 @@
       <c r="F5" s="4">
         <v>0.02</v>
       </c>
-      <c r="G5" s="4">
-        <v>0.05</v>
+      <c r="G5" s="6">
+        <v>0.04</v>
       </c>
       <c r="H5">
-        <v>6305</v>
+        <v>6360</v>
       </c>
       <c r="I5">
         <v>0.95</v>
@@ -2785,7 +2828,7 @@
         <v>0.05</v>
       </c>
       <c r="K5">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2807,8 +2850,8 @@
       <c r="F6" s="4">
         <v>0.06</v>
       </c>
-      <c r="G6" s="4">
-        <v>0.03</v>
+      <c r="G6" s="6">
+        <v>0.02</v>
       </c>
       <c r="H6">
         <v>454</v>
@@ -2820,7 +2863,7 @@
         <v>0.08</v>
       </c>
       <c r="K6">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2828,31 +2871,31 @@
         <v>25</v>
       </c>
       <c r="B7">
-        <v>309</v>
+        <v>3625</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="6">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>49</v>
+        <v>3352</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2863,34 +2906,34 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>6497</v>
+        <v>408570</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>0.74</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
+        <v>0.26</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.09</v>
       </c>
       <c r="H8">
-        <v>285</v>
+        <v>401366</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -2898,34 +2941,34 @@
         <v>27</v>
       </c>
       <c r="B9">
-        <v>17537</v>
+        <v>657809</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="D9" s="4">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="E9" s="4">
-        <v>1</v>
+        <v>0.69</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.18</v>
+        <v>0.31</v>
+      </c>
+      <c r="G9" s="6">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H9">
-        <v>1864</v>
+        <v>628431</v>
       </c>
       <c r="I9">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>0.42</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -2933,69 +2976,69 @@
         <v>28</v>
       </c>
       <c r="B10">
-        <v>22003</v>
+        <v>27082</v>
       </c>
       <c r="C10" s="4">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="D10" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="E10" s="4">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="F10" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="G10" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="G10" s="6">
         <v>0.01</v>
       </c>
       <c r="H10">
-        <v>1161</v>
+        <v>4635</v>
       </c>
       <c r="I10">
-        <v>0.91</v>
+        <v>0.96</v>
       </c>
       <c r="J10">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="K10">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11">
-        <v>13220</v>
+        <v>47565</v>
       </c>
       <c r="C11" s="4">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="D11" s="4">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="E11" s="4">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="F11" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.24</v>
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.01</v>
       </c>
       <c r="H11">
-        <v>1895</v>
+        <v>35681</v>
       </c>
       <c r="I11">
-        <v>0.97</v>
+        <v>0.93</v>
       </c>
       <c r="J11">
-        <v>0.03</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K11">
-        <v>1.07</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>